<commit_message>
Primer modelado. Separación de entidades obras y referentes
</commit_message>
<xml_diff>
--- a/datos/bga-metadatos.xlsx
+++ b/datos/bga-metadatos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemartin/HD/herramientas-digitales/modulo-db/bga-cat/iniciales/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/posgradosfacartes/Documents/repos/taller-docu/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C84285D-564C-6844-AEFC-B443140E0C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A98BD931-FB3E-8A46-9D82-4A50D62D22EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="33120" windowHeight="18400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="obra" sheetId="1" r:id="rId1"/>
+    <sheet name="referentes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Autor</t>
   </si>
@@ -52,18 +53,6 @@
   </si>
   <si>
     <t>Archivo</t>
-  </si>
-  <si>
-    <t>Título referente 2</t>
-  </si>
-  <si>
-    <t>Fecha ref 2</t>
-  </si>
-  <si>
-    <t>Periódico ref 2</t>
-  </si>
-  <si>
-    <t>Archivo ref 2</t>
   </si>
   <si>
     <t>Beatriz González</t>
@@ -554,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,12 +555,6 @@
     <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="8" width="43.5" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" customWidth="1"/>
-    <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1023" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -588,198 +571,217 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="AMI1"/>
     </row>
     <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:1023" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1">
-        <v>23922</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1023" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1">
-        <v>35209</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C5" s="6">
         <v>1969</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" s="6">
         <v>1969</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:1023" x14ac:dyDescent="0.2">
       <c r="C12" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7187323-E83D-A14A-A958-F3BC724908CA}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="43.5" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>23922</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <v>35209</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>